<commit_message>
Modifying test cases file
</commit_message>
<xml_diff>
--- a/Test Cases/Saucedemo - Test Automation .xlsx
+++ b/Test Cases/Saucedemo - Test Automation .xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="57">
   <si>
     <t>Action</t>
   </si>
@@ -28,81 +28,78 @@
     <t xml:space="preserve">Priority </t>
   </si>
   <si>
-    <t>iOS</t>
+    <t>Status</t>
   </si>
   <si>
     <t>Prereq.</t>
-  </si>
-  <si>
-    <t>Verify that login with a valid username and a valid password</t>
-  </si>
-  <si>
-    <t>High</t>
-  </si>
-  <si>
-    <t>1.1</t>
   </si>
   <si>
     <r>
       <rPr>
         <rFont val="Arial"/>
-        <sz val="10.0"/>
       </rPr>
       <t xml:space="preserve">Navigate to the website: </t>
     </r>
     <r>
       <rPr>
         <rFont val="Arial"/>
-        <color rgb="FF1155CC"/>
-        <sz val="10.0"/>
+        <color rgb="FF000000"/>
         <u/>
       </rPr>
-      <t>https://www.saucedemo.com</t>
+      <t xml:space="preserve">https://www.saucedemo.com
+</t>
     </r>
   </si>
   <si>
-    <t xml:space="preserve">The login page opens successfully </t>
-  </si>
-  <si>
-    <t>Ready to Test</t>
+    <t xml:space="preserve">The login page opens successfully
+ </t>
+  </si>
+  <si>
+    <t>Pass</t>
+  </si>
+  <si>
+    <t>Verify that login with a valid username and a valid password</t>
+  </si>
+  <si>
+    <t>High</t>
+  </si>
+  <si>
+    <t>1.1</t>
+  </si>
+  <si>
+    <t>Enter a valid username</t>
+  </si>
+  <si>
+    <t>the username entered to the username field</t>
+  </si>
+  <si>
+    <t>username: standard_user</t>
   </si>
   <si>
     <t>1.2</t>
   </si>
   <si>
-    <t>Enter a valid username</t>
-  </si>
-  <si>
-    <t>the username entered to the username field</t>
-  </si>
-  <si>
-    <t>username: standard_user</t>
+    <t>Enter a valid password</t>
+  </si>
+  <si>
+    <t>the password entered to the password field</t>
+  </si>
+  <si>
+    <t>password: secret_sauce</t>
   </si>
   <si>
     <t>1.3</t>
   </si>
   <si>
-    <t>Enter a valid password</t>
-  </si>
-  <si>
-    <t>the password entered to the password field</t>
-  </si>
-  <si>
-    <t>password: secret_sauce</t>
+    <t>Click on Login button</t>
+  </si>
+  <si>
+    <t>the button is clickable and the user redirects to products page</t>
   </si>
   <si>
     <t>1.4</t>
   </si>
   <si>
-    <t>Click on Login button</t>
-  </si>
-  <si>
-    <t>the button is clickable and the user redirects to products page</t>
-  </si>
-  <si>
-    <t>1.5</t>
-  </si>
-  <si>
     <t xml:space="preserve">Verify that the user logged in and redirects to products page successfully </t>
   </si>
   <si>
@@ -115,45 +112,24 @@
     <t>2.1</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <sz val="10.0"/>
-      </rPr>
-      <t xml:space="preserve">Navigate to the website: </t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <color rgb="FF1155CC"/>
-        <sz val="10.0"/>
-        <u/>
-      </rPr>
-      <t>https://www.saucedemo.com</t>
-    </r>
-  </si>
-  <si>
     <t>2.2</t>
   </si>
   <si>
+    <t>Enter an invalid password</t>
+  </si>
+  <si>
+    <t>password: ahmedali123</t>
+  </si>
+  <si>
     <t>2.3</t>
   </si>
   <si>
-    <t>Enter an invalid password</t>
-  </si>
-  <si>
-    <t>password: ahmedali123</t>
+    <t>the button is clickable and an error message appear conains "Epic sadface: Username and password do not match any user in this service"</t>
   </si>
   <si>
     <t>2.4</t>
   </si>
   <si>
-    <t>the button is clickable and an error message appear conains "Epic sadface: Username and password do not match any user in this service"</t>
-  </si>
-  <si>
-    <t>2.5</t>
-  </si>
-  <si>
     <t xml:space="preserve">the user blocked to log in </t>
   </si>
   <si>
@@ -163,42 +139,21 @@
     <t>3.1</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <sz val="10.0"/>
-      </rPr>
-      <t xml:space="preserve">Navigate to the website: </t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <color rgb="FF1155CC"/>
-        <sz val="10.0"/>
-        <u/>
-      </rPr>
-      <t>https://www.saucedemo.com</t>
-    </r>
+    <t>Enter an invalid username</t>
+  </si>
+  <si>
+    <t>username: ahmedali123</t>
   </si>
   <si>
     <t>3.2</t>
   </si>
   <si>
-    <t>Enter an invalid username</t>
-  </si>
-  <si>
-    <t>username: ahmedali123</t>
-  </si>
-  <si>
     <t>3.3</t>
   </si>
   <si>
     <t>3.4</t>
   </si>
   <si>
-    <t>3.5</t>
-  </si>
-  <si>
     <t>Verify that login with an invalid username and an invalid password</t>
   </si>
   <si>
@@ -208,24 +163,6 @@
     <t>4.1</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <sz val="10.0"/>
-      </rPr>
-      <t xml:space="preserve">Navigate to the website: </t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <color rgb="FF1155CC"/>
-        <sz val="10.0"/>
-        <u/>
-      </rPr>
-      <t>https://www.saucedemo.com</t>
-    </r>
-  </si>
-  <si>
     <t>4.2</t>
   </si>
   <si>
@@ -235,9 +172,6 @@
     <t>4.4</t>
   </si>
   <si>
-    <t>4.5</t>
-  </si>
-  <si>
     <t>Verify that login with leaving the username and password fields empty</t>
   </si>
   <si>
@@ -247,44 +181,22 @@
     <t>5.1</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <sz val="10.0"/>
-      </rPr>
-      <t xml:space="preserve">Navigate to the website: </t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <color rgb="FF1155CC"/>
-        <sz val="10.0"/>
-        <u/>
-      </rPr>
-      <t>https://www.saucedemo.com</t>
-    </r>
+    <t>Leave the username field empty</t>
   </si>
   <si>
     <t>5.2</t>
   </si>
   <si>
-    <t>Leave the username field empty</t>
+    <t>Leave the password field empty</t>
   </si>
   <si>
     <t>5.3</t>
   </si>
   <si>
-    <t>Leave the password field empty</t>
+    <t>the button is clickable and a validation message appears contians "Epic sadface: Username is required"</t>
   </si>
   <si>
     <t>5.4</t>
-  </si>
-  <si>
-    <t>the button is clickable and a validation message appears contians "Epic sadface: Username is required
-"</t>
-  </si>
-  <si>
-    <t>5.5</t>
   </si>
 </sst>
 </file>
@@ -294,7 +206,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="10">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -309,9 +221,17 @@
     </font>
     <font>
       <b/>
-      <sz val="12.0"/>
       <color rgb="FFFFFFFF"/>
-      <name val="Helvetica Neue"/>
+      <name val="&quot;Helvetica Neue&quot;"/>
+    </font>
+    <font>
+      <u/>
+      <color rgb="FF0000FF"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <color theme="1"/>
+      <name val="Arial"/>
     </font>
     <font>
       <sz val="10.0"/>
@@ -319,16 +239,10 @@
       <name val="Arial"/>
     </font>
     <font>
-      <u/>
-      <sz val="10.0"/>
-      <color rgb="FF0000FF"/>
-      <name val="Arial"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="10.0"/>
-      <color theme="10"/>
-      <name val="Arial"/>
+      <b/>
+      <sz val="12.0"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Helvetica Neue"/>
     </font>
     <font>
       <color theme="1"/>
@@ -336,8 +250,14 @@
       <scheme val="minor"/>
     </font>
     <font/>
+    <font>
+      <u/>
+      <sz val="10.0"/>
+      <color theme="10"/>
+      <name val="Arial"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -348,6 +268,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FF134F5C"/>
         <bgColor rgb="FF134F5C"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF76A5AF"/>
+        <bgColor rgb="FF76A5AF"/>
       </patternFill>
     </fill>
     <fill>
@@ -385,7 +311,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -398,47 +324,48 @@
     <xf borderId="1" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="1" fillId="3" fontId="2" numFmtId="1" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center" readingOrder="0" vertical="center"/>
+    <xf borderId="0" fillId="3" fontId="2" numFmtId="1" xfId="0" applyAlignment="1" applyFill="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf borderId="1" fillId="3" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="0" fillId="3" fontId="3" numFmtId="1" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="3" fontId="4" numFmtId="1" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="3" fontId="4" numFmtId="1" xfId="0" applyFont="1" applyNumberFormat="1"/>
+    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="1" fillId="4" fontId="6" numFmtId="1" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf borderId="1" fillId="4" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="1" fillId="3" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="1" fillId="4" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="1" fillId="3" fontId="2" numFmtId="1" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf borderId="1" fillId="5" fontId="5" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="1" fillId="4" fontId="3" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="1" fillId="4" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="1" fillId="5" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="1" fillId="4" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="5" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="1" fillId="4" fontId="3" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="4" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="2" fillId="4" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="2" fillId="3" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="3" fillId="0" fontId="7" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="0" fillId="4" fontId="3" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
+    <xf borderId="3" fillId="0" fontId="8" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="9" numFmtId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle xfId="0" name="Normal" builtinId="0"/>
@@ -690,12 +617,12 @@
   <cols>
     <col customWidth="1" min="1" max="1" width="7.88"/>
     <col customWidth="1" min="2" max="2" width="61.0"/>
-    <col customWidth="1" min="3" max="3" width="47.13"/>
-    <col customWidth="1" min="4" max="4" width="32.88"/>
+    <col customWidth="1" min="3" max="3" width="49.13"/>
+    <col customWidth="1" min="4" max="4" width="36.25"/>
     <col customWidth="1" min="5" max="5" width="20.88"/>
     <col customWidth="1" min="6" max="6" width="17.25"/>
     <col customWidth="1" min="7" max="7" width="14.25"/>
-    <col customWidth="1" min="8" max="24" width="12.75"/>
+    <col customWidth="1" min="8" max="26" width="12.75"/>
   </cols>
   <sheetData>
     <row r="1" ht="15.75" customHeight="1">
@@ -715,468 +642,505 @@
       <c r="F1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="3" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" ht="24.0" customHeight="1">
       <c r="A2" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="5"/>
-      <c r="C2" s="6"/>
-      <c r="D2" s="6"/>
-      <c r="E2" s="6"/>
-      <c r="F2" s="5"/>
-      <c r="G2" s="6"/>
+      <c r="B2" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" s="7"/>
+      <c r="F2" s="7"/>
+      <c r="G2" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="H2" s="7"/>
+      <c r="I2" s="9"/>
+      <c r="J2" s="9"/>
+      <c r="K2" s="9"/>
+      <c r="L2" s="9"/>
+      <c r="M2" s="9"/>
+      <c r="N2" s="9"/>
+      <c r="O2" s="9"/>
+      <c r="P2" s="9"/>
+      <c r="Q2" s="9"/>
+      <c r="R2" s="9"/>
+      <c r="S2" s="9"/>
+      <c r="T2" s="9"/>
+      <c r="U2" s="9"/>
+      <c r="V2" s="9"/>
+      <c r="W2" s="9"/>
+      <c r="X2" s="9"/>
+      <c r="Y2" s="9"/>
+      <c r="Z2" s="9"/>
     </row>
     <row r="3">
-      <c r="A3" s="7">
+      <c r="A3" s="10">
         <v>1.0</v>
       </c>
-      <c r="B3" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3" s="6"/>
-      <c r="D3" s="6"/>
-      <c r="E3" s="6"/>
-      <c r="F3" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="G3" s="6"/>
+      <c r="B3" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="12"/>
+      <c r="D3" s="12"/>
+      <c r="E3" s="12"/>
+      <c r="F3" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="G3" s="12"/>
     </row>
     <row r="4" ht="15.75" customHeight="1">
-      <c r="A4" s="8" t="s">
+      <c r="A4" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="E4" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="G4" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="C4" s="10" t="s">
+    </row>
+    <row r="5" ht="18.75" customHeight="1">
+      <c r="A5" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="C5" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="D5" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="E5" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="G5" s="8" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" ht="15.75" customHeight="1">
+      <c r="A6" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="B6" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="C6" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="D6" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="G6" s="8" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" ht="15.75" customHeight="1">
+      <c r="A7" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="B7" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="C7" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="D7" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="G7" s="8" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="10">
+        <v>2.0</v>
+      </c>
+      <c r="B8" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="C8" s="18"/>
+      <c r="D8" s="12"/>
+      <c r="E8" s="12"/>
+      <c r="F8" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="E4" s="11"/>
-      <c r="G4" s="12" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="5" ht="15.75" customHeight="1">
-      <c r="A5" s="8" t="s">
+      <c r="G8" s="12"/>
+    </row>
+    <row r="9" ht="15.75" customHeight="1">
+      <c r="A9" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="B9" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="10" t="s">
+      <c r="C9" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="C5" s="10" t="s">
+      <c r="D9" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="E9" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="E5" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="G5" s="12" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="6" ht="18.75" customHeight="1">
-      <c r="A6" s="8" t="s">
+      <c r="G9" s="8" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10" ht="15.75" customHeight="1">
+      <c r="A10" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="B10" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="C10" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="D10" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="E10" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="G10" s="8" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" ht="50.25" customHeight="1">
+      <c r="A11" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="B11" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="C11" s="16" t="s">
+        <v>32</v>
+      </c>
+      <c r="D11" s="16" t="s">
+        <v>32</v>
+      </c>
+      <c r="G11" s="8" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" ht="15.75" customHeight="1">
+      <c r="A12" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="B12" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="C12" s="16" t="s">
+        <v>34</v>
+      </c>
+      <c r="D12" s="16" t="s">
+        <v>34</v>
+      </c>
+      <c r="G12" s="8" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="13" ht="15.75" customHeight="1">
+      <c r="A13" s="10">
+        <v>3.0</v>
+      </c>
+      <c r="B13" s="17" t="s">
+        <v>35</v>
+      </c>
+      <c r="C13" s="18"/>
+      <c r="D13" s="12"/>
+      <c r="E13" s="12"/>
+      <c r="F13" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="G13" s="12"/>
+    </row>
+    <row r="14" ht="24.75" customHeight="1">
+      <c r="A14" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="B14" s="14" t="s">
+        <v>37</v>
+      </c>
+      <c r="C14" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="D14" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="E14" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="G14" s="8" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="15" ht="21.0" customHeight="1">
+      <c r="A15" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="B15" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="B6" s="10" t="s">
+      <c r="C15" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="C6" s="10" t="s">
+      <c r="D15" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="E15" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="E6" s="13" t="s">
-        <v>20</v>
-      </c>
-      <c r="G6" s="12" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="7" ht="15.75" customHeight="1">
-      <c r="A7" s="14" t="s">
+      <c r="G15" s="8" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="16" ht="51.0" customHeight="1">
+      <c r="A16" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="B16" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="B7" s="15" t="s">
-        <v>22</v>
-      </c>
-      <c r="C7" s="15" t="s">
-        <v>23</v>
-      </c>
-      <c r="G7" s="12"/>
-    </row>
-    <row r="8" ht="15.75" customHeight="1">
-      <c r="A8" s="14" t="s">
+      <c r="C16" s="16" t="s">
+        <v>32</v>
+      </c>
+      <c r="D16" s="16" t="s">
+        <v>32</v>
+      </c>
+      <c r="G16" s="8" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="17" ht="15.75" customHeight="1">
+      <c r="A17" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="B17" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="B8" s="15" t="s">
-        <v>25</v>
-      </c>
-      <c r="C8" s="15" t="s">
-        <v>26</v>
-      </c>
-      <c r="G8" s="12"/>
-    </row>
-    <row r="9">
-      <c r="A9" s="7">
-        <v>2.0</v>
-      </c>
-      <c r="B9" s="16" t="s">
-        <v>27</v>
-      </c>
-      <c r="C9" s="17"/>
-      <c r="D9" s="6"/>
-      <c r="E9" s="6"/>
-      <c r="F9" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="G9" s="6"/>
-    </row>
-    <row r="10" ht="15.75" customHeight="1">
-      <c r="A10" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="B10" s="9" t="s">
+      <c r="C17" s="16" t="s">
+        <v>34</v>
+      </c>
+      <c r="D17" s="16" t="s">
+        <v>34</v>
+      </c>
+      <c r="G17" s="8" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="18" ht="15.75" customHeight="1">
+      <c r="A18" s="10">
+        <v>4.0</v>
+      </c>
+      <c r="B18" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="C18" s="18"/>
+      <c r="D18" s="12"/>
+      <c r="E18" s="12"/>
+      <c r="F18" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="G18" s="12"/>
+    </row>
+    <row r="19" ht="24.75" customHeight="1">
+      <c r="A19" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="B19" s="14" t="s">
+        <v>37</v>
+      </c>
+      <c r="C19" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="D19" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="E19" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="G19" s="8" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="20" ht="25.5" customHeight="1">
+      <c r="A20" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="B20" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="C10" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="G10" s="12" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="11" ht="15.75" customHeight="1">
-      <c r="A11" s="8" t="s">
+      <c r="C20" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="D20" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="E20" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="B11" s="10" t="s">
+      <c r="G20" s="8" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="21" ht="60.0" customHeight="1">
+      <c r="A21" s="13" t="s">
+        <v>46</v>
+      </c>
+      <c r="B21" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="C21" s="16" t="s">
+        <v>32</v>
+      </c>
+      <c r="D21" s="16" t="s">
+        <v>32</v>
+      </c>
+      <c r="G21" s="8" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="22" ht="15.75" customHeight="1">
+      <c r="A22" s="13" t="s">
+        <v>47</v>
+      </c>
+      <c r="B22" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="C22" s="16" t="s">
+        <v>34</v>
+      </c>
+      <c r="D22" s="16" t="s">
+        <v>34</v>
+      </c>
+      <c r="G22" s="8" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="23" ht="15.75" customHeight="1">
+      <c r="A23" s="10">
+        <v>5.0</v>
+      </c>
+      <c r="B23" s="17" t="s">
+        <v>48</v>
+      </c>
+      <c r="C23" s="18"/>
+      <c r="D23" s="12"/>
+      <c r="E23" s="12"/>
+      <c r="F23" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="G23" s="12"/>
+    </row>
+    <row r="24" ht="30.0" customHeight="1">
+      <c r="A24" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="B24" s="14" t="s">
+        <v>51</v>
+      </c>
+      <c r="C24" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="C11" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="E11" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="G11" s="12" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="12" ht="15.75" customHeight="1">
-      <c r="A12" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="B12" s="10" t="s">
-        <v>32</v>
-      </c>
-      <c r="C12" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="E12" s="13" t="s">
-        <v>33</v>
-      </c>
-      <c r="G12" s="12" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="13" ht="50.25" customHeight="1">
-      <c r="A13" s="14" t="s">
+      <c r="D24" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="G24" s="8" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="25" ht="19.5" customHeight="1">
+      <c r="A25" s="13" t="s">
+        <v>52</v>
+      </c>
+      <c r="B25" s="14" t="s">
+        <v>53</v>
+      </c>
+      <c r="C25" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="D25" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="G25" s="8" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="26" ht="44.25" customHeight="1">
+      <c r="A26" s="13" t="s">
+        <v>54</v>
+      </c>
+      <c r="B26" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="C26" s="16" t="s">
+        <v>55</v>
+      </c>
+      <c r="D26" s="16" t="s">
+        <v>55</v>
+      </c>
+      <c r="G26" s="8" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="27" ht="15.75" customHeight="1">
+      <c r="A27" s="13" t="s">
+        <v>56</v>
+      </c>
+      <c r="B27" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="C27" s="16" t="s">
         <v>34</v>
       </c>
-      <c r="B13" s="15" t="s">
-        <v>22</v>
-      </c>
-      <c r="C13" s="15" t="s">
-        <v>35</v>
-      </c>
-      <c r="G13" s="12"/>
-    </row>
-    <row r="14" ht="15.75" customHeight="1">
-      <c r="A14" s="14" t="s">
-        <v>36</v>
-      </c>
-      <c r="B14" s="15" t="s">
-        <v>25</v>
-      </c>
-      <c r="C14" s="15" t="s">
-        <v>37</v>
-      </c>
-      <c r="G14" s="12"/>
-    </row>
-    <row r="15" ht="15.75" customHeight="1">
-      <c r="A15" s="7">
-        <v>3.0</v>
-      </c>
-      <c r="B15" s="16" t="s">
-        <v>38</v>
-      </c>
-      <c r="C15" s="17"/>
-      <c r="D15" s="6"/>
-      <c r="E15" s="6"/>
-      <c r="F15" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="G15" s="6"/>
-    </row>
-    <row r="16" ht="15.75" customHeight="1">
-      <c r="A16" s="8" t="s">
-        <v>39</v>
-      </c>
-      <c r="B16" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="C16" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="G16" s="12" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="17" ht="24.75" customHeight="1">
-      <c r="A17" s="8" t="s">
-        <v>41</v>
-      </c>
-      <c r="B17" s="10" t="s">
-        <v>42</v>
-      </c>
-      <c r="C17" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="E17" s="13" t="s">
-        <v>43</v>
-      </c>
-      <c r="G17" s="12" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="18" ht="21.0" customHeight="1">
-      <c r="A18" s="8" t="s">
-        <v>44</v>
-      </c>
-      <c r="B18" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="C18" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="E18" s="13" t="s">
-        <v>20</v>
-      </c>
-      <c r="G18" s="12" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="19" ht="51.0" customHeight="1">
-      <c r="A19" s="14" t="s">
-        <v>45</v>
-      </c>
-      <c r="B19" s="15" t="s">
-        <v>22</v>
-      </c>
-      <c r="C19" s="15" t="s">
-        <v>35</v>
-      </c>
-      <c r="G19" s="12"/>
-    </row>
-    <row r="20" ht="15.75" customHeight="1">
-      <c r="A20" s="14" t="s">
-        <v>46</v>
-      </c>
-      <c r="B20" s="15" t="s">
-        <v>25</v>
-      </c>
-      <c r="C20" s="15" t="s">
-        <v>37</v>
-      </c>
-      <c r="G20" s="12"/>
-    </row>
-    <row r="21" ht="15.75" customHeight="1">
-      <c r="A21" s="7">
-        <v>4.0</v>
-      </c>
-      <c r="B21" s="16" t="s">
-        <v>47</v>
-      </c>
-      <c r="C21" s="17"/>
-      <c r="D21" s="6"/>
-      <c r="E21" s="6"/>
-      <c r="F21" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="G21" s="6"/>
-    </row>
-    <row r="22" ht="15.75" customHeight="1">
-      <c r="A22" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="B22" s="9" t="s">
-        <v>50</v>
-      </c>
-      <c r="C22" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="G22" s="12" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="23" ht="24.75" customHeight="1">
-      <c r="A23" s="8" t="s">
-        <v>51</v>
-      </c>
-      <c r="B23" s="10" t="s">
-        <v>42</v>
-      </c>
-      <c r="C23" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="E23" s="13" t="s">
-        <v>43</v>
-      </c>
-      <c r="G23" s="12" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="24" ht="25.5" customHeight="1">
-      <c r="A24" s="8" t="s">
-        <v>52</v>
-      </c>
-      <c r="B24" s="10" t="s">
-        <v>32</v>
-      </c>
-      <c r="C24" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="E24" s="13" t="s">
-        <v>33</v>
-      </c>
-      <c r="G24" s="12" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="25" ht="47.25" customHeight="1">
-      <c r="A25" s="14" t="s">
-        <v>53</v>
-      </c>
-      <c r="B25" s="15" t="s">
-        <v>22</v>
-      </c>
-      <c r="C25" s="15" t="s">
-        <v>35</v>
-      </c>
-      <c r="G25" s="12"/>
-    </row>
-    <row r="26" ht="15.75" customHeight="1">
-      <c r="A26" s="14" t="s">
-        <v>54</v>
-      </c>
-      <c r="B26" s="15" t="s">
-        <v>25</v>
-      </c>
-      <c r="C26" s="15" t="s">
-        <v>37</v>
-      </c>
-      <c r="G26" s="12"/>
-    </row>
-    <row r="27" ht="15.75" customHeight="1">
-      <c r="A27" s="7">
-        <v>5.0</v>
-      </c>
-      <c r="B27" s="16" t="s">
-        <v>55</v>
-      </c>
-      <c r="C27" s="17"/>
-      <c r="D27" s="6"/>
-      <c r="E27" s="6"/>
-      <c r="F27" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="G27" s="6"/>
+      <c r="D27" s="16" t="s">
+        <v>34</v>
+      </c>
+      <c r="G27" s="8" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="28" ht="15.75" customHeight="1">
-      <c r="A28" s="8" t="s">
-        <v>57</v>
-      </c>
-      <c r="B28" s="9" t="s">
-        <v>58</v>
-      </c>
-      <c r="C28" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="G28" s="12" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="29" ht="18.75" customHeight="1">
-      <c r="A29" s="8" t="s">
-        <v>59</v>
-      </c>
-      <c r="B29" s="10" t="s">
-        <v>60</v>
-      </c>
-      <c r="C29" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="G29" s="12" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="30" ht="19.5" customHeight="1">
-      <c r="A30" s="14" t="s">
-        <v>61</v>
-      </c>
-      <c r="B30" s="10" t="s">
-        <v>62</v>
-      </c>
-      <c r="C30" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="G30" s="12" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="31" ht="44.25" customHeight="1">
-      <c r="A31" s="14" t="s">
-        <v>63</v>
-      </c>
-      <c r="B31" s="15" t="s">
-        <v>22</v>
-      </c>
-      <c r="C31" s="15" t="s">
-        <v>64</v>
-      </c>
-      <c r="G31" s="12" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="32" ht="15.75" customHeight="1">
-      <c r="A32" s="18" t="s">
-        <v>65</v>
-      </c>
-      <c r="B32" s="15" t="s">
-        <v>25</v>
-      </c>
-      <c r="C32" s="15" t="s">
-        <v>37</v>
-      </c>
-      <c r="G32" s="12" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="33" ht="15.75" customHeight="1">
-      <c r="A33" s="7"/>
-      <c r="B33" s="16"/>
-      <c r="C33" s="17"/>
-      <c r="D33" s="6"/>
-      <c r="E33" s="6"/>
-      <c r="F33" s="5"/>
-      <c r="G33" s="6"/>
-    </row>
+      <c r="A28" s="10"/>
+      <c r="B28" s="17"/>
+      <c r="C28" s="18"/>
+      <c r="D28" s="12"/>
+      <c r="E28" s="12"/>
+      <c r="F28" s="11"/>
+      <c r="G28" s="12"/>
+    </row>
+    <row r="29" ht="15.75" customHeight="1"/>
+    <row r="30" ht="15.75" customHeight="1">
+      <c r="E30" s="19"/>
+    </row>
+    <row r="31" ht="15.75" customHeight="1"/>
+    <row r="32" ht="15.75" customHeight="1"/>
+    <row r="33" ht="15.75" customHeight="1"/>
     <row r="34" ht="15.75" customHeight="1"/>
-    <row r="35" ht="15.75" customHeight="1">
-      <c r="E35" s="11"/>
-    </row>
+    <row r="35" ht="15.75" customHeight="1"/>
     <row r="36" ht="15.75" customHeight="1"/>
     <row r="37" ht="15.75" customHeight="1"/>
     <row r="38" ht="15.75" customHeight="1"/>
@@ -2121,49 +2085,40 @@
     <row r="977" ht="15.75" customHeight="1"/>
     <row r="978" ht="15.75" customHeight="1"/>
     <row r="979" ht="15.75" customHeight="1"/>
-    <row r="980" ht="15.75" customHeight="1"/>
-    <row r="981" ht="15.75" customHeight="1"/>
-    <row r="982" ht="15.75" customHeight="1"/>
-    <row r="983" ht="15.75" customHeight="1"/>
-    <row r="984" ht="15.75" customHeight="1"/>
   </sheetData>
   <mergeCells count="5">
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="B15:C15"/>
-    <mergeCell ref="B21:C21"/>
-    <mergeCell ref="B27:C27"/>
-    <mergeCell ref="B33:C33"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="B23:C23"/>
+    <mergeCell ref="B28:C28"/>
   </mergeCells>
-  <conditionalFormatting sqref="G4:G8 G10:G14 G16:G20 G22:G26 G28:G32">
+  <conditionalFormatting sqref="G2 G4:G7 G9:G12 G14:G17 G19:G22 G24:G27">
     <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="Pass">
-      <formula>NOT(ISERROR(SEARCH(("Pass"),(G4))))</formula>
+      <formula>NOT(ISERROR(SEARCH(("Pass"),(G2))))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G4:G8 G10:G14 G16:G20 G22:G26 G28:G32">
+  <conditionalFormatting sqref="G2 G4:G7 G9:G12 G14:G17 G19:G22 G24:G27">
     <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="Fail">
-      <formula>NOT(ISERROR(SEARCH(("Fail"),(G4))))</formula>
+      <formula>NOT(ISERROR(SEARCH(("Fail"),(G2))))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G4:G8 G10:G14 G16:G20 G22:G26 G28:G32">
+  <conditionalFormatting sqref="G2 G4:G7 G9:G12 G14:G17 G19:G22 G24:G27">
     <cfRule type="containsText" dxfId="2" priority="3" operator="containsText" text="Block / Skip">
-      <formula>NOT(ISERROR(SEARCH(("Block / Skip"),(G4))))</formula>
+      <formula>NOT(ISERROR(SEARCH(("Block / Skip"),(G2))))</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="G4:G8 G10:G14 G16:G20 G22:G26 G28:G32">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="G2 G4:G7 G9:G12 G14:G17 G19:G22 G24:G27">
       <formula1>"Ready to Test,Pass,Fail,Block / Skip"</formula1>
     </dataValidation>
   </dataValidations>
   <hyperlinks>
-    <hyperlink r:id="rId1" ref="B4"/>
-    <hyperlink r:id="rId2" ref="B10"/>
-    <hyperlink r:id="rId3" ref="B16"/>
-    <hyperlink r:id="rId4" ref="B22"/>
-    <hyperlink r:id="rId5" ref="B28"/>
+    <hyperlink r:id="rId1" ref="B2"/>
   </hyperlinks>
   <printOptions/>
   <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
   <pageSetup orientation="landscape"/>
-  <drawing r:id="rId6"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>